<commit_message>
Push of my completed work for group project.
</commit_message>
<xml_diff>
--- a/Project Research Outline.xlsx
+++ b/Project Research Outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a8333f12ef70eba/Desktop/FINTECH_Bootcamp/Project/Fintech_Project_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{B36A795D-8C19-412D-912F-367EE499FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBD79E1B-EF72-4472-9581-49D19F93E999}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{B36A795D-8C19-412D-912F-367EE499FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5577827A-3A0E-4B8E-ACDD-6DEC124389A5}"/>
   <bookViews>
-    <workbookView xWindow="34020" yWindow="2100" windowWidth="17280" windowHeight="8970" xr2:uid="{A1C22619-2114-4AC0-ADE4-6CFD64AF2143}"/>
+    <workbookView xWindow="29355" yWindow="240" windowWidth="26580" windowHeight="10200" xr2:uid="{A1C22619-2114-4AC0-ADE4-6CFD64AF2143}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Stocks</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>Parrallel Coordinates</t>
-  </si>
-  <si>
-    <t>Up for Grabs</t>
   </si>
   <si>
     <t>compare</t>
@@ -576,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F175470E-BD86-4903-9422-BEBF9575F8CC}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,7 +603,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -633,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -658,7 +655,7 @@
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -720,10 +717,10 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
         <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -747,7 +744,7 @@
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -771,7 +768,7 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>30</v>
@@ -798,7 +795,7 @@
         <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -806,7 +803,7 @@
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -814,7 +811,7 @@
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -829,8 +826,9 @@
     <hyperlink ref="H5" r:id="rId4" xr:uid="{12ED872C-A272-4D46-81D7-E913AA0B920A}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{8E8C1C4D-86AF-4DE2-B1F3-D1577A976EDB}"/>
     <hyperlink ref="F5" r:id="rId6" xr:uid="{D5CD7377-13E4-4D9F-8B75-4DA65236320E}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{75A13912-C6DA-4F3D-B3E2-74B77370C452}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>